<commit_message>
added Extent Spark Report and PDF report.
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/postmorbidity.xlsx
+++ b/src/test/resources/exceldata/postmorbidity.xlsx
@@ -607,9 +607,7 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -624,9 +622,7 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
+      <c r="E3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -641,9 +637,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -658,9 +652,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
+      <c r="E5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -675,9 +667,7 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
+      <c r="E6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -692,9 +682,7 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
+      <c r="E7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -709,9 +697,7 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -726,9 +712,7 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -743,9 +727,7 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -760,9 +742,7 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
+      <c r="E11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -813,9 +793,7 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>55</v>
-      </c>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -830,9 +808,7 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -847,9 +823,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -864,9 +838,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
+      <c r="E5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -881,9 +853,7 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>59</v>
-      </c>
+      <c r="E6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>